<commit_message>
REFRESH INFO EXCEL viernes 04
</commit_message>
<xml_diff>
--- a/assets/data/enruedate2019.xlsx
+++ b/assets/data/enruedate2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNO\Documents\arcela43.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89150185-DE4F-4A76-9534-1F103BE75069}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635B38C0-F2D3-44F2-879D-749ED925F037}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="949" xr2:uid="{CFA91A2F-D3C5-4056-901E-5E58B99EF3EB}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="212">
   <si>
     <t>PAREJAS GUAGUANCO</t>
   </si>
@@ -174,12 +174,6 @@
     <t>PASION LATINA</t>
   </si>
   <si>
-    <t>GABRIEL - REBECA</t>
-  </si>
-  <si>
-    <t>SANDUGA</t>
-  </si>
-  <si>
     <t>GABRIEL - EGLIMAR</t>
   </si>
   <si>
@@ -225,15 +219,9 @@
     <t>A&amp;A</t>
   </si>
   <si>
-    <t>JEFFERSON MACSENE</t>
-  </si>
-  <si>
     <t>MIGUEL VILLALOBOS</t>
   </si>
   <si>
-    <t>ISBEL ROBLES</t>
-  </si>
-  <si>
     <t>EDWARD LANDAEZ</t>
   </si>
   <si>
@@ -697,6 +685,9 @@
   </si>
   <si>
     <t>GENERO ADICONAL</t>
+  </si>
+  <si>
+    <t>JONATHAN ABOUD</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1397,6 +1388,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1448,28 +1463,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1786,10 +1786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F680A068-AF74-4DC7-A18B-610ACE22163B}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,25 +1800,23 @@
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="49"/>
-    </row>
-    <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+    </row>
+    <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1838,194 +1836,148 @@
         <v>5</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="7">
-        <f>SUM(F3:K3)</f>
-        <v>0</v>
+        <f>SUM(F3:J3)</f>
+        <v>36</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I3" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J3" s="7">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D7" si="0">SUM(F4:K4)</f>
-        <v>0</v>
+        <f>SUM(F4:J4)</f>
+        <v>31</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G4" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I4" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(F5:J5)</f>
+        <v>29</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G5" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H5" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
-        <v>0</v>
-      </c>
-      <c r="J6" s="9">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="B6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="11">
+        <f>SUM(F6:J6)</f>
+        <v>29</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11">
+        <v>7</v>
+      </c>
+      <c r="G6" s="11">
+        <v>6</v>
+      </c>
+      <c r="H6" s="11">
+        <v>6</v>
+      </c>
+      <c r="I6" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11">
-        <v>0</v>
-      </c>
-      <c r="I7" s="11">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11">
-        <v>0</v>
+      <c r="J6" s="11">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J6">
+    <sortCondition descending="1" ref="D3:D6"/>
+  </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2053,30 +2005,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2107,15 +2059,15 @@
         <v>10</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="7">
         <f>SUM(F3:M3)</f>
         <v>0</v>
@@ -2150,8 +2102,8 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="58"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D12" si="0">SUM(F4:M4)</f>
         <v>0</v>
@@ -2186,8 +2138,8 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2222,8 +2174,8 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2258,8 +2210,8 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2294,8 +2246,8 @@
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2330,8 +2282,8 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2366,8 +2318,8 @@
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2402,8 +2354,8 @@
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2438,8 +2390,8 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2511,22 +2463,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2578,7 +2530,7 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:N3)</f>
@@ -2992,21 +2944,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3054,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>39</v>
@@ -3094,7 +3046,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>39</v>
@@ -3134,10 +3086,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -3174,10 +3126,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -3214,10 +3166,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -3254,10 +3206,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -3294,10 +3246,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -3334,10 +3286,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
@@ -3374,10 +3326,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
@@ -3414,10 +3366,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
@@ -3454,10 +3406,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
@@ -3494,7 +3446,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>39</v>
@@ -3559,21 +3511,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3621,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>39</v>
@@ -3661,10 +3613,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -3700,10 +3652,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D5" s="9">
         <v>0</v>
@@ -3739,10 +3691,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D6" s="9">
         <v>0</v>
@@ -3778,10 +3730,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7" s="9">
         <v>0</v>
@@ -3817,10 +3769,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D8" s="9">
         <v>0</v>
@@ -3856,7 +3808,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>39</v>
@@ -3920,21 +3872,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3982,10 +3934,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:M3)</f>
@@ -4022,10 +3974,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D8" si="0">SUM(F4:M4)</f>
@@ -4062,10 +4014,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -4102,10 +4054,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -4142,10 +4094,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -4182,10 +4134,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
@@ -4245,20 +4197,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4303,10 +4255,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
@@ -4340,10 +4292,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D12" si="0">SUM(F4:L4)</f>
@@ -4377,10 +4329,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -4414,10 +4366,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -4451,10 +4403,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -4488,10 +4440,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -4525,10 +4477,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -4562,10 +4514,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
@@ -4599,10 +4551,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
@@ -4636,10 +4588,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
@@ -4700,29 +4652,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4757,8 +4709,8 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -4790,8 +4742,8 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="58"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D12" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -4823,8 +4775,8 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4856,8 +4808,8 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4889,8 +4841,8 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4922,8 +4874,8 @@
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4955,8 +4907,8 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4988,8 +4940,8 @@
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5021,8 +4973,8 @@
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5054,8 +5006,8 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5124,20 +5076,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5182,10 +5134,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
@@ -5219,10 +5171,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D15" si="0">SUM(F4:L4)</f>
@@ -5256,10 +5208,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -5293,10 +5245,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -5330,10 +5282,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -5367,10 +5319,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -5404,10 +5356,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -5441,10 +5393,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
@@ -5478,10 +5430,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
@@ -5515,10 +5467,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
@@ -5552,10 +5504,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
@@ -5589,10 +5541,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
@@ -5626,10 +5578,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
@@ -5687,20 +5639,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5745,10 +5697,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
@@ -5782,10 +5734,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D15" si="0">SUM(F4:L4)</f>
@@ -5819,10 +5771,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -5856,10 +5808,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -5893,10 +5845,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -5930,10 +5882,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -5967,10 +5919,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -6004,10 +5956,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
@@ -6041,10 +5993,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
@@ -6078,10 +6030,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
@@ -6115,10 +6067,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
@@ -6152,10 +6104,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
@@ -6189,10 +6141,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
@@ -6250,29 +6202,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -6307,10 +6259,10 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="56"/>
+      <c r="B3" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="64"/>
       <c r="D3" s="15">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -6342,10 +6294,10 @@
       <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="58"/>
+      <c r="B4" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="66"/>
       <c r="D4" s="16">
         <f t="shared" ref="D4:D7" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -6377,10 +6329,10 @@
       <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="58"/>
+      <c r="B5" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="66"/>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6412,10 +6364,10 @@
       <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="58"/>
+      <c r="B6" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="66"/>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6447,10 +6399,10 @@
       <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="51"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6494,39 +6446,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D3B04C-C77B-48A6-913A-E5F52797CF8D}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="3" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="49"/>
-    </row>
-    <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+    </row>
+    <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6546,33 +6496,30 @@
         <v>5</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="7">
-        <f>SUM(F3:K3)</f>
+        <v>129</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="15">
+        <f>SUM(F3:J3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -6591,22 +6538,19 @@
       <c r="J3" s="7">
         <v>0</v>
       </c>
-      <c r="K3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="9">
-        <f t="shared" ref="D4:D12" si="0">SUM(F4:K4)</f>
+        <v>121</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="16">
+        <f>SUM(F4:J4)</f>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -6625,22 +6569,19 @@
       <c r="J4" s="9">
         <v>0</v>
       </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="9">
-        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(F5:J5)</f>
         <v>0</v>
       </c>
       <c r="E5" s="9"/>
@@ -6659,22 +6600,19 @@
       <c r="J5" s="9">
         <v>0</v>
       </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="9">
-        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="16">
+        <f>SUM(F6:J6)</f>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -6693,22 +6631,19 @@
       <c r="J6" s="9">
         <v>0</v>
       </c>
-      <c r="K6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="9">
-        <f t="shared" si="0"/>
+      <c r="C7" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="16">
+        <f>SUM(F7:J7)</f>
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
@@ -6727,22 +6662,19 @@
       <c r="J7" s="9">
         <v>0</v>
       </c>
-      <c r="K7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="9">
-        <f t="shared" si="0"/>
+        <v>211</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="16">
+        <f>SUM(F8:J8)</f>
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
@@ -6761,22 +6693,19 @@
       <c r="J8" s="9">
         <v>0</v>
       </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="9">
-        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="16">
+        <f>SUM(F9:J9)</f>
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
@@ -6795,22 +6724,19 @@
       <c r="J9" s="9">
         <v>0</v>
       </c>
-      <c r="K9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="9">
-        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="16">
+        <f>SUM(F10:J10)</f>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -6829,22 +6755,19 @@
       <c r="J10" s="9">
         <v>0</v>
       </c>
-      <c r="K10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="9">
-        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="16">
+        <f>SUM(F11:J11)</f>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -6863,47 +6786,72 @@
       <c r="J11" s="9">
         <v>0</v>
       </c>
-      <c r="K11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11">
-        <v>0</v>
-      </c>
-      <c r="G12" s="11">
-        <v>0</v>
-      </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
-        <v>0</v>
-      </c>
-      <c r="J12" s="11">
-        <v>0</v>
-      </c>
-      <c r="K12" s="11">
+      <c r="D12" s="16">
+        <f>SUM(F12:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="17">
+        <f>SUM(F13:J13)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6930,20 +6878,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6988,10 +6936,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
@@ -7025,10 +6973,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D11" si="0">SUM(F4:L4)</f>
@@ -7063,7 +7011,7 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -7097,10 +7045,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -7134,10 +7082,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -7171,10 +7119,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -7209,7 +7157,7 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -7243,10 +7191,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
@@ -7280,10 +7228,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D11" s="11">
         <f t="shared" si="0"/>
@@ -7342,21 +7290,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7404,10 +7352,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:M3)</f>
@@ -7444,10 +7392,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D15" si="0">SUM(F4:M4)</f>
@@ -7484,10 +7432,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -7524,10 +7472,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -7564,10 +7512,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -7604,10 +7552,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -7644,10 +7592,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D9" s="9">
         <f>SUM(F9:M9)</f>
@@ -7684,10 +7632,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" ref="D10:D12" si="1">SUM(F10:M10)</f>
@@ -7724,10 +7672,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="1"/>
@@ -7764,10 +7712,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="1"/>
@@ -7804,10 +7752,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
@@ -7844,10 +7792,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
@@ -7884,10 +7832,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
@@ -7947,19 +7895,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8001,7 +7949,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>39</v>
@@ -8035,7 +7983,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>39</v>
@@ -8069,7 +8017,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>39</v>
@@ -8103,7 +8051,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>39</v>
@@ -8137,7 +8085,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>39</v>
@@ -8171,7 +8119,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>39</v>
@@ -8205,10 +8153,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D9" s="21">
         <f t="shared" si="0"/>
@@ -8239,10 +8187,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D10" s="21">
         <f t="shared" si="0"/>
@@ -8273,10 +8221,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D11" s="21">
         <f t="shared" si="0"/>
@@ -8307,10 +8255,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12" s="21">
         <f t="shared" si="0"/>
@@ -8341,10 +8289,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D13" s="21">
         <f>SUM(F13:K13)</f>
@@ -8375,10 +8323,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D14" s="21">
         <f t="shared" ref="D14:D18" si="1">SUM(F14:K14)</f>
@@ -8409,10 +8357,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D15" s="21">
         <f t="shared" si="1"/>
@@ -8443,10 +8391,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D16" s="21">
         <f t="shared" si="1"/>
@@ -8477,10 +8425,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D17" s="21">
         <f t="shared" si="1"/>
@@ -8511,7 +8459,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>39</v>
@@ -8568,29 +8516,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -8625,10 +8573,10 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="56"/>
+      <c r="B3" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="64"/>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -8660,10 +8608,10 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="58"/>
+      <c r="B4" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="66"/>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D7" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -8695,10 +8643,10 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="58"/>
+      <c r="B5" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="66"/>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8730,10 +8678,10 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="58"/>
+      <c r="B6" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="66"/>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8765,10 +8713,10 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="51"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8831,29 +8779,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -8888,10 +8836,10 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="56"/>
+      <c r="B3" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="64"/>
       <c r="D3" s="15">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -8923,10 +8871,10 @@
       <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="58"/>
+      <c r="B4" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="66"/>
       <c r="D4" s="16">
         <f t="shared" ref="D4:D7" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -8958,10 +8906,10 @@
       <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="58"/>
+      <c r="B5" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="66"/>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8993,10 +8941,10 @@
       <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="58"/>
+      <c r="B6" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="66"/>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -9028,10 +8976,10 @@
       <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="51"/>
+      <c r="B7" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="59"/>
       <c r="D7" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -9095,22 +9043,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9161,10 +9109,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="7">
         <f>SUM(F3:N3)</f>
@@ -9204,7 +9152,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>39</v>
@@ -9247,7 +9195,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>39</v>
@@ -9290,10 +9238,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -9333,10 +9281,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -9376,7 +9324,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>39</v>
@@ -9443,27 +9391,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -9501,7 +9449,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>39</v>
@@ -9538,10 +9486,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D16" si="0">SUM(F4:L4)</f>
@@ -9575,10 +9523,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -9612,10 +9560,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -9649,10 +9597,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -9686,10 +9634,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -9723,10 +9671,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -9760,10 +9708,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
@@ -9797,10 +9745,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
@@ -9834,10 +9782,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
@@ -9871,10 +9819,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
@@ -9908,10 +9856,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
@@ -9945,10 +9893,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="0"/>
@@ -9982,7 +9930,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>39</v>
@@ -10042,27 +9990,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -10100,7 +10048,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>39</v>
@@ -10137,10 +10085,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D10" si="0">SUM(F4:L4)</f>
@@ -10174,10 +10122,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -10211,10 +10159,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -10248,10 +10196,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -10286,7 +10234,7 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -10320,10 +10268,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -10357,7 +10305,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>39</v>
@@ -10417,29 +10365,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="71"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -10474,10 +10422,10 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="56"/>
+      <c r="B3" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="64"/>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -10509,10 +10457,10 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="58"/>
+      <c r="B4" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="66"/>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D6" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -10544,10 +10492,10 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="58"/>
+      <c r="B5" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="66"/>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -10579,10 +10527,10 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="51"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -10645,21 +10593,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -10707,9 +10655,9 @@
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="51" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="7">
@@ -10747,10 +10695,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="69" t="s">
-        <v>61</v>
+        <v>97</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>57</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D12" si="0">SUM(F4:M4)</f>
@@ -10787,10 +10735,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="69" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>98</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
@@ -10827,10 +10775,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>66</v>
+        <v>100</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>62</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
@@ -10867,10 +10815,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="69" t="s">
-        <v>94</v>
+        <v>101</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>90</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
@@ -10907,10 +10855,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="69" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>103</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
@@ -10947,10 +10895,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>58</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
@@ -10987,10 +10935,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>66</v>
+        <v>105</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>62</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
@@ -11027,10 +10975,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>107</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
@@ -11067,10 +11015,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="69" t="s">
-        <v>102</v>
+        <v>108</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>98</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
@@ -11107,37 +11055,37 @@
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>89</v>
+        <v>109</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>85</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
       </c>
       <c r="E13" s="40"/>
-      <c r="F13" s="64">
-        <v>0</v>
-      </c>
-      <c r="G13" s="64">
-        <v>0</v>
-      </c>
-      <c r="H13" s="64">
-        <v>0</v>
-      </c>
-      <c r="I13" s="64">
-        <v>0</v>
-      </c>
-      <c r="J13" s="64">
-        <v>0</v>
-      </c>
-      <c r="K13" s="64">
-        <v>0</v>
-      </c>
-      <c r="L13" s="64">
-        <v>0</v>
-      </c>
-      <c r="M13" s="65">
+      <c r="F13" s="47">
+        <v>0</v>
+      </c>
+      <c r="G13" s="47">
+        <v>0</v>
+      </c>
+      <c r="H13" s="47">
+        <v>0</v>
+      </c>
+      <c r="I13" s="47">
+        <v>0</v>
+      </c>
+      <c r="J13" s="47">
+        <v>0</v>
+      </c>
+      <c r="K13" s="47">
+        <v>0</v>
+      </c>
+      <c r="L13" s="47">
+        <v>0</v>
+      </c>
+      <c r="M13" s="48">
         <v>0</v>
       </c>
     </row>
@@ -11146,37 +11094,37 @@
         <v>12</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="54" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="11">
         <v>0</v>
       </c>
       <c r="E14" s="41"/>
-      <c r="F14" s="66">
-        <v>0</v>
-      </c>
-      <c r="G14" s="66">
-        <v>0</v>
-      </c>
-      <c r="H14" s="66">
-        <v>0</v>
-      </c>
-      <c r="I14" s="66">
-        <v>0</v>
-      </c>
-      <c r="J14" s="66">
-        <v>0</v>
-      </c>
-      <c r="K14" s="66">
-        <v>0</v>
-      </c>
-      <c r="L14" s="66">
-        <v>0</v>
-      </c>
-      <c r="M14" s="67">
+      <c r="F14" s="49">
+        <v>0</v>
+      </c>
+      <c r="G14" s="49">
+        <v>0</v>
+      </c>
+      <c r="H14" s="49">
+        <v>0</v>
+      </c>
+      <c r="I14" s="49">
+        <v>0</v>
+      </c>
+      <c r="J14" s="49">
+        <v>0</v>
+      </c>
+      <c r="K14" s="49">
+        <v>0</v>
+      </c>
+      <c r="L14" s="49">
+        <v>0</v>
+      </c>
+      <c r="M14" s="50">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
REFRESH INFO EXCEL sabado 05-10
</commit_message>
<xml_diff>
--- a/assets/data/enruedate2019.xlsx
+++ b/assets/data/enruedate2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNO\Documents\arcela43.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4776F2F1-F618-4E8A-AE65-15274B344DE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A5DC7-4AA4-40A4-81A5-A8109AB73ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="949" firstSheet="9" activeTab="14" xr2:uid="{CFA91A2F-D3C5-4056-901E-5E58B99EF3EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="949" firstSheet="13" activeTab="15" xr2:uid="{CFA91A2F-D3C5-4056-901E-5E58B99EF3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="PAREJAS GUAGUANCO" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="200">
   <si>
     <t>PAREJAS GUAGUANCO</t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t>TUMBAO CARIBE</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1398,6 +1401,27 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1449,24 +1473,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1798,18 +1850,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1998,21 +2050,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2096,7 +2148,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="68">
+      <c r="A4" s="52">
         <v>2</v>
       </c>
       <c r="B4" s="19" t="s">
@@ -2105,16 +2157,16 @@
       <c r="C4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -2157,7 +2209,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="68">
+      <c r="A6" s="52">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -2237,7 +2289,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="68">
+      <c r="A8" s="52">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -2317,7 +2369,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="68">
+      <c r="A10" s="52">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2397,7 +2449,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="68">
+      <c r="A12" s="52">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -2477,7 +2529,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="71">
+      <c r="A14" s="55">
         <v>12</v>
       </c>
       <c r="B14" s="30" t="s">
@@ -2546,21 +2598,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2907,21 +2959,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3177,7 +3229,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3193,20 +3245,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3620,10 +3672,10 @@
       <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="51" t="s">
         <v>179</v>
       </c>
       <c r="D13" s="9">
@@ -3719,29 +3771,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="63" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3776,10 +3828,10 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -3811,10 +3863,10 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D5" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -3846,10 +3898,10 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3893,7 +3945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB712281-00E1-4FDC-A84D-5C48720B0CEB}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -3911,20 +3963,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3975,7 +4027,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="7">
-        <f>SUM(F3:L3)</f>
+        <f t="shared" ref="D3:D13" si="0">SUM(F3:L3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -4012,7 +4064,7 @@
         <v>198</v>
       </c>
       <c r="D4" s="9">
-        <f>SUM(F4:L4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -4049,7 +4101,7 @@
         <v>115</v>
       </c>
       <c r="D5" s="9">
-        <f>SUM(F5:L5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" s="9"/>
@@ -4086,7 +4138,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="9">
-        <f>SUM(F6:L6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -4123,7 +4175,7 @@
         <v>198</v>
       </c>
       <c r="D7" s="9">
-        <f>SUM(F7:L7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
@@ -4160,7 +4212,7 @@
         <v>115</v>
       </c>
       <c r="D8" s="9">
-        <f>SUM(F8:L8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
@@ -4197,7 +4249,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="9">
-        <f>SUM(F9:L9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
@@ -4234,7 +4286,7 @@
         <v>53</v>
       </c>
       <c r="D10" s="9">
-        <f>SUM(F10:L10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -4271,7 +4323,7 @@
         <v>120</v>
       </c>
       <c r="D11" s="9">
-        <f>SUM(F11:L11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -4308,7 +4360,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="9">
-        <f>SUM(F12:L12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" s="9"/>
@@ -4345,7 +4397,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="11">
-        <f>SUM(F13:L13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" s="11"/>
@@ -4383,7 +4435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D675C796-FBE0-4A3C-AE52-1F243CD1E14C}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
@@ -4400,20 +4452,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4464,7 +4516,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="7">
-        <f>SUM(F3:L3)</f>
+        <f t="shared" ref="D3:D12" si="0">SUM(F3:L3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -4501,7 +4553,7 @@
         <v>120</v>
       </c>
       <c r="D4" s="9">
-        <f>SUM(F4:L4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -4538,7 +4590,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="9">
-        <f>SUM(F5:L5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" s="9"/>
@@ -4575,7 +4627,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="9">
-        <f>SUM(F6:L6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -4612,7 +4664,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="9">
-        <f>SUM(F7:L7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
@@ -4649,7 +4701,7 @@
         <v>55</v>
       </c>
       <c r="D8" s="9">
-        <f>SUM(F8:L8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
@@ -4686,7 +4738,7 @@
         <v>77</v>
       </c>
       <c r="D9" s="9">
-        <f>SUM(F9:L9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
@@ -4723,7 +4775,7 @@
         <v>53</v>
       </c>
       <c r="D10" s="9">
-        <f>SUM(F10:L10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -4760,7 +4812,7 @@
         <v>120</v>
       </c>
       <c r="D11" s="9">
-        <f>SUM(F11:L11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -4797,7 +4849,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="11">
-        <f>SUM(F12:L12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" s="11"/>
@@ -4852,29 +4904,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="63" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4909,10 +4961,10 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="15">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -4944,10 +4996,10 @@
       <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="16">
         <f t="shared" ref="D4:D6" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -4979,10 +5031,10 @@
       <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5014,10 +5066,10 @@
       <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="52"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5063,7 +5115,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5079,20 +5131,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5230,14 +5282,14 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="54" t="s">
         <v>197</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>135</v>
       </c>
       <c r="D6" s="9">
-        <f>SUM(F6:L6)</f>
+        <f t="shared" ref="D6:D11" si="0">SUM(F6:L6)</f>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -5274,7 +5326,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="9">
-        <f>SUM(F7:L7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
@@ -5311,7 +5363,7 @@
         <v>135</v>
       </c>
       <c r="D8" s="9">
-        <f>SUM(F8:L8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
@@ -5348,7 +5400,7 @@
         <v>140</v>
       </c>
       <c r="D9" s="9">
-        <f>SUM(F9:L9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
@@ -5385,7 +5437,7 @@
         <v>136</v>
       </c>
       <c r="D10" s="9">
-        <f>SUM(F10:L10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -5422,7 +5474,7 @@
         <v>71</v>
       </c>
       <c r="D11" s="9">
-        <f>SUM(F11:L11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -5449,7 +5501,7 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="70"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="8"/>
     </row>
   </sheetData>
@@ -5483,21 +5535,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5551,7 +5603,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="7">
-        <f>SUM(F3:M3)</f>
+        <f t="shared" ref="D3:D9" si="0">SUM(F3:M3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -5591,7 +5643,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="9">
-        <f>SUM(F4:M4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -5631,7 +5683,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="9">
-        <f>SUM(F5:M5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" s="9"/>
@@ -5671,7 +5723,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="9">
-        <f>SUM(F6:M6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -5711,7 +5763,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="9">
-        <f>SUM(F7:M7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
@@ -5751,7 +5803,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="9">
-        <f>SUM(F8:M8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
@@ -5791,7 +5843,7 @@
         <v>55</v>
       </c>
       <c r="D9" s="9">
-        <f>SUM(F9:M9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
@@ -5831,7 +5883,7 @@
         <v>194</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" ref="D10:D11" si="0">SUM(F10:M10)</f>
+        <f t="shared" ref="D10:D11" si="1">SUM(F10:M10)</f>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -5871,7 +5923,7 @@
         <v>190</v>
       </c>
       <c r="D11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -6087,18 +6139,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6505,19 +6557,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6565,7 +6617,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="7">
-        <f>SUM(F3:K3)</f>
+        <f t="shared" ref="D3:D16" si="0">SUM(F3:K3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -6599,7 +6651,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="9">
-        <f>SUM(F4:K4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -6633,7 +6685,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="9">
-        <f>SUM(F5:K5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" s="9"/>
@@ -6667,7 +6719,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="9">
-        <f>SUM(F6:K6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -6701,7 +6753,7 @@
         <v>36</v>
       </c>
       <c r="D7" s="9">
-        <f>SUM(F7:K7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
@@ -6735,7 +6787,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="9">
-        <f>SUM(F8:K8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
@@ -6769,7 +6821,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="9">
-        <f>SUM(F9:K9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
@@ -6803,7 +6855,7 @@
         <v>53</v>
       </c>
       <c r="D10" s="9">
-        <f>SUM(F10:K10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -6837,7 +6889,7 @@
         <v>51</v>
       </c>
       <c r="D11" s="9">
-        <f>SUM(F11:K11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -6871,7 +6923,7 @@
         <v>154</v>
       </c>
       <c r="D12" s="9">
-        <f>SUM(F12:K12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" s="9"/>
@@ -6905,7 +6957,7 @@
         <v>53</v>
       </c>
       <c r="D13" s="9">
-        <f>SUM(F13:K13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" s="9"/>
@@ -6939,7 +6991,7 @@
         <v>50</v>
       </c>
       <c r="D14" s="9">
-        <f>SUM(F14:K14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14" s="9"/>
@@ -6973,7 +7025,7 @@
         <v>73</v>
       </c>
       <c r="D15" s="9">
-        <f>SUM(F15:K15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E15" s="9"/>
@@ -7007,7 +7059,7 @@
         <v>36</v>
       </c>
       <c r="D16" s="11">
-        <f>SUM(F16:K16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16" s="11"/>
@@ -7043,7 +7095,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7058,32 +7110,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="82" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -7115,10 +7167,12 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="58"/>
+      <c r="B3" s="79" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>199</v>
+      </c>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -7150,10 +7204,12 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="80" t="s">
+        <v>199</v>
+      </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D7" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -7185,10 +7241,12 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="80" t="s">
+        <v>199</v>
+      </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7220,10 +7278,12 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="60"/>
+      <c r="C6" s="80" t="s">
+        <v>199</v>
+      </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7255,10 +7315,12 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="52"/>
+      <c r="C7" s="78" t="s">
+        <v>199</v>
+      </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7287,14 +7349,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7305,7 +7361,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7321,29 +7377,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="87" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="74" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -7378,10 +7434,12 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="88" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="58"/>
       <c r="D3" s="15">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -7413,10 +7471,12 @@
       <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="88" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="60"/>
       <c r="D4" s="16">
         <f t="shared" ref="D4:D6" si="0">SUM(F4:L4)</f>
         <v>0</v>
@@ -7448,10 +7508,12 @@
       <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="88" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="60"/>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7483,10 +7545,12 @@
       <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="88" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="52"/>
       <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7515,13 +7579,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7549,22 +7608,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="61"/>
     </row>
     <row r="2" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7897,20 +7956,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8065,10 +8124,10 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="50" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="9">
@@ -8496,20 +8555,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8784,7 +8843,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8799,29 +8858,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="65"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="72"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="73" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="74" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -8856,10 +8915,12 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="75" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="75" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="58"/>
       <c r="D3" s="7">
         <f>SUM(F3:L3)</f>
         <v>0</v>
@@ -8888,31 +8949,35 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="68">
+      <c r="A4" s="52">
         <v>2</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="75" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="76" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="60"/>
       <c r="D5" s="9">
         <f t="shared" ref="D5:D7" si="0">SUM(F5:L5)</f>
         <v>0</v>
@@ -8944,10 +9009,12 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="76" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="60"/>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8979,10 +9046,12 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="52"/>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -9011,14 +9080,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9046,21 +9109,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
REFRESH INFO EXCEL domingo 06-10
</commit_message>
<xml_diff>
--- a/assets/data/enruedate2019.xlsx
+++ b/assets/data/enruedate2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNO\Documents\arcela43.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E6720F-6E30-4D67-8002-7461A28ADA84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75D87FF-7250-4513-8E3E-33D4C4D99D7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="949" firstSheet="11" activeTab="11" xr2:uid="{CFA91A2F-D3C5-4056-901E-5E58B99EF3EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="949" firstSheet="11" activeTab="13" xr2:uid="{CFA91A2F-D3C5-4056-901E-5E58B99EF3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="PAREJAS GUAGUANCO" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="199">
   <si>
     <t>PAREJAS GUAGUANCO</t>
   </si>
@@ -966,7 +966,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1215,96 +1215,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1450,11 +1360,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1513,13 +1443,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1536,16 +1466,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1584,7 +1514,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1601,11 +1531,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1642,16 +1572,16 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1669,7 +1599,7 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1678,7 +1608,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1687,7 +1617,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1696,50 +1626,53 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3266,8 +3199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB0B8C-5748-4965-8F02-4BA9CCB48CA3}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3332,16 +3265,16 @@
         <v>9</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>195</v>
@@ -3352,39 +3285,39 @@
         <v>1</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C3" s="55" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="7">
-        <f>F3+G3+H3+I3+J3+K3+L3+M3-N3</f>
-        <v>0</v>
+        <f>F3+G3+H3+I3+L3+M3+J3+K3-N3</f>
+        <v>73</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J3" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L3" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N3" s="7">
         <v>0</v>
@@ -3395,39 +3328,39 @@
         <v>2</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D7" si="0">F4+G4+H4+I4+J4+K4+L4+M4-N4</f>
-        <v>0</v>
+        <f>F4+G4+H4+I4+L4+M4+J4+K4-N4</f>
+        <v>71</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J4" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K4" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L4" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N4" s="9">
         <v>0</v>
@@ -3438,39 +3371,39 @@
         <v>3</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="56" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>F5+G5+H5+I5+L5+M5+J5+K5-N5</f>
+        <v>61</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G5" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H5" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I5" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J5" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K5" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L5" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M5" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N5" s="9">
         <v>0</v>
@@ -3481,39 +3414,39 @@
         <v>4</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D6" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>F6+G6+H6+I6+L6+M6+J6+K6-N6</f>
+        <v>52</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H6" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I6" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J6" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K6" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L6" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M6" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N6" s="9">
         <v>0</v>
@@ -3524,45 +3457,48 @@
         <v>5</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="D7" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>F7+G7+H7+I7+L7+M7+J7+K7-N7</f>
+        <v>48</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11">
         <v>0</v>
       </c>
       <c r="G7" s="11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H7" s="11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I7" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J7" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K7" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L7" s="11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M7" s="11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N7" s="11">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N7">
+    <sortCondition descending="1" ref="D3:D7"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:N1"/>
   </mergeCells>
@@ -3575,7 +3511,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3589,7 +3525,7 @@
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -3611,449 +3547,449 @@
       <c r="L1" s="85"/>
       <c r="M1" s="85"/>
     </row>
-    <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="G2" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="67" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" s="96" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="15">
-        <f>F3+G3+H3+I3+J3+K3+L3-M3</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
-        <v>0</v>
+        <v>104</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="7">
+        <f>F3+G3+H3+I3+K3+L3+J3-M3</f>
+        <v>69</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="100">
+        <v>10</v>
       </c>
       <c r="G3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J3" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M3" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="9">
+        <f>F4+G4+H4+I4+K4+L4+J4-M4</f>
+        <v>69</v>
+      </c>
+      <c r="E4" s="99"/>
+      <c r="F4" s="9">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9">
+        <v>10</v>
+      </c>
+      <c r="H4" s="9">
+        <v>10</v>
+      </c>
+      <c r="I4" s="9">
+        <v>10</v>
+      </c>
+      <c r="J4" s="9">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9">
+        <v>10</v>
+      </c>
+      <c r="L4" s="9">
+        <v>10</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="97" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="30">
+        <f>F5+G5+H5+I5+K5+L5+J5-M5</f>
+        <v>63</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="30">
+        <v>10</v>
+      </c>
+      <c r="G5" s="30">
+        <v>9</v>
+      </c>
+      <c r="H5" s="30">
+        <v>9</v>
+      </c>
+      <c r="I5" s="98">
+        <v>10</v>
+      </c>
+      <c r="J5" s="30">
+        <v>9</v>
+      </c>
+      <c r="K5" s="30">
+        <v>8</v>
+      </c>
+      <c r="L5" s="30">
+        <v>8</v>
+      </c>
+      <c r="M5" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="9">
+        <f>F6+G6+H6+I6+K6+L6+J6-M6</f>
+        <v>63</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="9">
+        <v>10</v>
+      </c>
+      <c r="G6" s="9">
+        <v>9</v>
+      </c>
+      <c r="H6" s="9">
+        <v>9</v>
+      </c>
+      <c r="I6" s="9">
+        <v>9</v>
+      </c>
+      <c r="J6" s="9">
+        <v>10</v>
+      </c>
+      <c r="K6" s="9">
+        <v>8</v>
+      </c>
+      <c r="L6" s="9">
+        <v>8</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="9">
+        <f>F7+G7+H7+I7+K7+L7+J7-M7</f>
+        <v>62</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="9">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9">
+        <v>9</v>
+      </c>
+      <c r="H7" s="9">
+        <v>9</v>
+      </c>
+      <c r="I7" s="9">
+        <v>9</v>
+      </c>
+      <c r="J7" s="9">
+        <v>9</v>
+      </c>
+      <c r="K7" s="9">
+        <v>8</v>
+      </c>
+      <c r="L7" s="9">
+        <v>8</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="9">
+        <f>F8+G8+H8+I8+K8+L8+J8-M8</f>
+        <v>60</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="9">
+        <v>10</v>
+      </c>
+      <c r="G8" s="9">
+        <v>7</v>
+      </c>
+      <c r="H8" s="69">
+        <v>10</v>
+      </c>
+      <c r="I8" s="9">
+        <v>9</v>
+      </c>
+      <c r="J8" s="9">
+        <v>9</v>
+      </c>
+      <c r="K8" s="9">
+        <v>8</v>
+      </c>
+      <c r="L8" s="9">
+        <v>7</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="9">
+        <f>F9+G9+H9+I9+K9+L9+J9-M9</f>
+        <v>60</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="9">
+        <v>9</v>
+      </c>
+      <c r="I9" s="9">
+        <v>9</v>
+      </c>
+      <c r="J9" s="9">
+        <v>9</v>
+      </c>
+      <c r="K9" s="9">
+        <v>8</v>
+      </c>
+      <c r="L9" s="9">
+        <v>7</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="9">
+        <f>F10+G10+H10+I10+K10+L10+J10-M10</f>
+        <v>59</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="9">
+        <v>10</v>
+      </c>
+      <c r="G10" s="9">
+        <v>9</v>
+      </c>
+      <c r="H10" s="9">
+        <v>8</v>
+      </c>
+      <c r="I10" s="9">
+        <v>8</v>
+      </c>
+      <c r="J10" s="9">
+        <v>9</v>
+      </c>
+      <c r="K10" s="9">
+        <v>7</v>
+      </c>
+      <c r="L10" s="9">
+        <v>8</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="9">
+        <f>F11+G11+H11+I11+K11+L11+J11-M11</f>
+        <v>58</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="9">
+        <v>10</v>
+      </c>
+      <c r="G11" s="9">
+        <v>9</v>
+      </c>
+      <c r="H11" s="9">
+        <v>8</v>
+      </c>
+      <c r="I11" s="9">
+        <v>8</v>
+      </c>
+      <c r="J11" s="9">
+        <v>9</v>
+      </c>
+      <c r="K11" s="69">
+        <v>7</v>
+      </c>
+      <c r="L11" s="9">
+        <v>7</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C12" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="16">
-        <f t="shared" ref="D4:D14" si="0">F4+G4+H4+I4+J4+K4+L4-M4</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>3</v>
-      </c>
-      <c r="B5" s="56" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
-        <v>0</v>
-      </c>
-      <c r="G5" s="9">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9">
-        <v>0</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0</v>
-      </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>4</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>173</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
-        <v>0</v>
-      </c>
-      <c r="J6" s="9">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
-        <v>0</v>
-      </c>
-      <c r="L6" s="9">
-        <v>0</v>
-      </c>
-      <c r="M6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>5</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="97" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
-        <v>0</v>
-      </c>
-      <c r="L7" s="9">
-        <v>0</v>
-      </c>
-      <c r="M7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>6</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="97" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9">
-        <v>0</v>
-      </c>
-      <c r="M8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>7</v>
-      </c>
-      <c r="B9" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="97" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>8</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="97" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9">
-        <v>0</v>
-      </c>
-      <c r="M10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>9</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="97" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
-        <v>0</v>
-      </c>
-      <c r="J11" s="9">
-        <v>0</v>
-      </c>
-      <c r="K11" s="9">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>10</v>
-      </c>
-      <c r="B12" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="97" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="9"/>
+      <c r="D12" s="9">
+        <f>F12+G12+H12+I12+K12+L12+J12-M12</f>
+        <v>58</v>
+      </c>
+      <c r="E12" s="16"/>
       <c r="F12" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G12" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H12" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I12" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J12" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K12" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L12" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M12" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="56" t="s">
@@ -4062,81 +3998,85 @@
       <c r="C13" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="9"/>
+      <c r="D13" s="9">
+        <f>F13+G13+H13+I13+K13+L13+J13-M13</f>
+        <v>57</v>
+      </c>
+      <c r="E13" s="16"/>
       <c r="F13" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G13" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H13" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I13" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J13" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K13" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L13" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M13" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="98" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="11"/>
+        <v>176</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="11">
+        <f>F14+G14+H14+I14+K14+L14+J14-M14</f>
+        <v>49</v>
+      </c>
+      <c r="E14" s="17"/>
       <c r="F14" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G14" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H14" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I14" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J14" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K14" s="11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L14" s="11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M14" s="11">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M14">
+    <sortCondition descending="1" ref="D3:D14"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4144,8 +4084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6972AB4-548C-46E5-AFA4-85F08BF384BD}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,10 +4124,10 @@
       <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="87" t="s">
         <v>192</v>
       </c>
       <c r="D2" s="54" t="s">
@@ -4209,13 +4149,13 @@
         <v>9</v>
       </c>
       <c r="J2" s="67" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K2" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="67" t="s">
         <v>32</v>
-      </c>
-      <c r="L2" s="67" t="s">
-        <v>10</v>
       </c>
       <c r="M2" s="67" t="s">
         <v>195</v>
@@ -4232,30 +4172,30 @@
         <v>192</v>
       </c>
       <c r="D3" s="7">
-        <f>F3+G3+H3+I3+J3+K3+L3-M3</f>
-        <v>0</v>
+        <f>F3+G3+H3+I3+K3+L3+J3-M3</f>
+        <v>48</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K3" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L3" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M3" s="7">
         <v>0</v>
@@ -4272,7 +4212,7 @@
         <v>192</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D5" si="0">F4+G4+H4+I4+J4+K4+L4-M4</f>
+        <f>F4+G4+H4+I4+K4+L4+J4-M4</f>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -4312,7 +4252,7 @@
         <v>192</v>
       </c>
       <c r="D5" s="11">
-        <f t="shared" si="0"/>
+        <f>F5+G5+H5+I5+K5+L5+J5-M5</f>
         <v>0</v>
       </c>
       <c r="E5" s="11"/>
@@ -4354,7 +4294,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,7 +4333,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="88" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="58" t="s">
@@ -4883,13 +4823,14 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
@@ -5371,19 +5312,22 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5401,16 +5345,17 @@
       <c r="J1" s="85"/>
       <c r="K1" s="85"/>
       <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="87" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>3</v>
+        <v>192</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -5447,12 +5392,14 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="91"/>
+      <c r="C3" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="D3" s="15">
-        <f>SUM(F3:L3)</f>
+        <f>F3+G3+H3+I3+J3+K3+L3-M3</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -5475,6 +5422,9 @@
         <v>0</v>
       </c>
       <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
         <v>0</v>
       </c>
     </row>
@@ -5482,12 +5432,14 @@
       <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="39" t="s">
+        <v>192</v>
+      </c>
       <c r="D4" s="16">
-        <f t="shared" ref="D4:D6" si="0">SUM(F4:L4)</f>
+        <f t="shared" ref="D4:D6" si="0">F4+G4+H4+I4+J4+K4+L4-M4</f>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -5510,6 +5462,9 @@
         <v>0</v>
       </c>
       <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
         <v>0</v>
       </c>
     </row>
@@ -5517,10 +5472,12 @@
       <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="93"/>
+      <c r="C5" s="39" t="s">
+        <v>192</v>
+      </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5545,6 +5502,9 @@
         <v>0</v>
       </c>
       <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
         <v>0</v>
       </c>
     </row>
@@ -5552,10 +5512,12 @@
       <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="87"/>
+      <c r="C6" s="35" t="s">
+        <v>192</v>
+      </c>
       <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5582,15 +5544,13 @@
       <c r="L6" s="11">
         <v>0</v>
       </c>
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5601,45 +5561,49 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="80"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
     </row>
     <row r="2" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="58" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -5661,30 +5625,30 @@
         <v>9</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="7">
-        <f>SUM(F3:L3)</f>
+      <c r="D3" s="15">
+        <f>F3+G3+H3+I3+J3+K3+L3-M3</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -5709,19 +5673,22 @@
       <c r="L3" s="7">
         <v>0</v>
       </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="91" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="9">
-        <f>SUM(F4:L4)</f>
+      <c r="D4" s="16">
+        <f t="shared" ref="D4:D11" si="0">F4+G4+H4+I4+J4+K4+L4-M4</f>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -5746,39 +5713,62 @@
       <c r="L4" s="9">
         <v>0</v>
       </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="91" t="s">
         <v>178</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="92" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="9">
-        <f t="shared" ref="D6:D11" si="0">SUM(F6:L6)</f>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -5803,18 +5793,21 @@
       <c r="L6" s="9">
         <v>0</v>
       </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="91" t="s">
         <v>133</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5840,18 +5833,21 @@
       <c r="L7" s="9">
         <v>0</v>
       </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="25" t="s">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" s="91" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5877,18 +5873,21 @@
       <c r="L8" s="9">
         <v>0</v>
       </c>
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5914,18 +5913,21 @@
       <c r="L9" s="9">
         <v>0</v>
       </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="25" t="s">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="91" t="s">
         <v>177</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5951,18 +5953,21 @@
       <c r="L10" s="9">
         <v>0</v>
       </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>9</v>
-      </c>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="14">
+        <v>9</v>
+      </c>
+      <c r="B11" s="93" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5986,6 +5991,9 @@
         <v>0</v>
       </c>
       <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
         <v>0</v>
       </c>
     </row>
@@ -5995,7 +6003,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6006,39 +6014,42 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D4" sqref="D4:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="80"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
     </row>
     <row r="2" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6085,17 +6096,17 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="7">
-        <f t="shared" ref="D3:D9" si="0">SUM(F3:M3)</f>
+      <c r="D3" s="15">
+        <f>F3+G3+H3+I3+J3+K3+L3+M3-N3</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -6123,19 +6134,22 @@
       <c r="M3" s="7">
         <v>0</v>
       </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="91" t="s">
         <v>140</v>
       </c>
       <c r="C4" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="9">
-        <f t="shared" si="0"/>
+      <c r="D4" s="16">
+        <f t="shared" ref="D4:D15" si="0">F4+G4+H4+I4+J4+K4+L4+M4-N4</f>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -6163,18 +6177,21 @@
       <c r="M4" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="N4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="91" t="s">
         <v>141</v>
       </c>
       <c r="C5" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6203,18 +6220,21 @@
       <c r="M5" s="9">
         <v>0</v>
       </c>
+      <c r="N5" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="91" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6243,18 +6263,21 @@
       <c r="M6" s="9">
         <v>0</v>
       </c>
+      <c r="N6" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="91" t="s">
         <v>138</v>
       </c>
       <c r="C7" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6283,18 +6306,21 @@
       <c r="M7" s="9">
         <v>0</v>
       </c>
+      <c r="N7" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="56" t="s">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" s="91" t="s">
         <v>179</v>
       </c>
       <c r="C8" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6323,18 +6349,21 @@
       <c r="M8" s="9">
         <v>0</v>
       </c>
+      <c r="N8" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="56" t="s">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="91" t="s">
         <v>142</v>
       </c>
       <c r="C9" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6363,19 +6392,22 @@
       <c r="M9" s="9">
         <v>0</v>
       </c>
+      <c r="N9" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="56" t="s">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="91" t="s">
         <v>186</v>
       </c>
       <c r="C10" s="56" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="9">
-        <f t="shared" ref="D10:D11" si="1">SUM(F10:M10)</f>
+      <c r="D10" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -6403,19 +6435,22 @@
       <c r="M10" s="9">
         <v>0</v>
       </c>
+      <c r="N10" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="56" t="s">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="91" t="s">
         <v>182</v>
       </c>
       <c r="C11" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="D11" s="9">
-        <f t="shared" si="1"/>
+      <c r="D11" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -6443,19 +6478,22 @@
       <c r="M11" s="9">
         <v>0</v>
       </c>
+      <c r="N11" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="56" t="s">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="91" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="9">
-        <f>SUM(F12:M12)</f>
+      <c r="D12" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" s="9"/>
@@ -6483,19 +6521,22 @@
       <c r="M12" s="9">
         <v>0</v>
       </c>
+      <c r="N12" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="91" t="s">
         <v>144</v>
       </c>
       <c r="C13" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="9">
-        <f>SUM(F13:M13)</f>
+      <c r="D13" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" s="9"/>
@@ -6523,19 +6564,22 @@
       <c r="M13" s="9">
         <v>0</v>
       </c>
+      <c r="N13" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="91" t="s">
         <v>145</v>
       </c>
       <c r="C14" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="D14" s="9">
-        <f>SUM(F14:M14)</f>
+      <c r="D14" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14" s="9"/>
@@ -6563,19 +6607,22 @@
       <c r="M14" s="9">
         <v>0</v>
       </c>
+      <c r="N14" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="A15" s="14">
         <v>13</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="93" t="s">
         <v>146</v>
       </c>
       <c r="C15" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="11">
-        <f>SUM(F15:M15)</f>
+      <c r="D15" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E15" s="11"/>
@@ -6603,10 +6650,13 @@
       <c r="M15" s="11">
         <v>0</v>
       </c>
+      <c r="N15" s="11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7034,7 +7084,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7044,36 +7094,38 @@
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="80"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="58" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -7100,22 +7152,22 @@
       <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="94" t="s">
+      <c r="L2" s="86" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="7">
-        <f>SUM(F3:K3)</f>
+      <c r="D3" s="15">
+        <f>F3+G3+H3+I3+J3+K3-L3</f>
         <v>0</v>
       </c>
       <c r="E3" s="7"/>
@@ -7137,19 +7189,22 @@
       <c r="K3" s="7">
         <v>0</v>
       </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="9">
-        <f>SUM(F4:K4)</f>
+      <c r="D4" s="16">
+        <f t="shared" ref="D4:D16" si="0">F4+G4+H4+I4+J4+K4-L4</f>
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
@@ -7171,19 +7226,22 @@
       <c r="K4" s="9">
         <v>0</v>
       </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="9">
-        <f>SUM(F5:K5)</f>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" s="9"/>
@@ -7205,19 +7263,22 @@
       <c r="K5" s="9">
         <v>0</v>
       </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="9">
-        <f>SUM(F6:K6)</f>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
@@ -7239,19 +7300,22 @@
       <c r="K6" s="9">
         <v>0</v>
       </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="9">
-        <f>SUM(F7:K7)</f>
+      <c r="D7" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
@@ -7273,19 +7337,22 @@
       <c r="K7" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" s="91" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="9">
-        <f>SUM(F8:K8)</f>
+      <c r="D8" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
@@ -7307,19 +7374,22 @@
       <c r="K8" s="9">
         <v>0</v>
       </c>
+      <c r="L8" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="9">
-        <f>SUM(F9:K9)</f>
+      <c r="D9" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
@@ -7341,19 +7411,22 @@
       <c r="K9" s="9">
         <v>0</v>
       </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="91" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="9">
-        <f>SUM(F10:K10)</f>
+      <c r="D10" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
@@ -7375,19 +7448,22 @@
       <c r="K10" s="9">
         <v>0</v>
       </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="91" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="9">
-        <f>SUM(F11:K11)</f>
+      <c r="D11" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="9"/>
@@ -7409,19 +7485,22 @@
       <c r="K11" s="9">
         <v>0</v>
       </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="D12" s="9">
-        <f>SUM(F12:K12)</f>
+      <c r="D12" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" s="9"/>
@@ -7443,19 +7522,22 @@
       <c r="K12" s="9">
         <v>0</v>
       </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="9">
-        <f>SUM(F13:K13)</f>
+      <c r="D13" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" s="9"/>
@@ -7477,19 +7559,22 @@
       <c r="K13" s="9">
         <v>0</v>
       </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="9">
-        <f>SUM(F14:K14)</f>
+      <c r="D14" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14" s="9"/>
@@ -7511,19 +7596,22 @@
       <c r="K14" s="9">
         <v>0</v>
       </c>
+      <c r="L14" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="13">
         <v>13</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="9">
-        <f>SUM(F15:K15)</f>
+      <c r="D15" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E15" s="9"/>
@@ -7545,19 +7633,22 @@
       <c r="K15" s="9">
         <v>0</v>
       </c>
+      <c r="L15" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="14">
         <v>14</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="11">
-        <f>SUM(F16:K16)</f>
+      <c r="D16" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16" s="11"/>
@@ -7579,10 +7670,13 @@
       <c r="K16" s="11">
         <v>0</v>
       </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>